<commit_message>
[Update] Review first 10 problems
</commit_message>
<xml_diff>
--- a/LeetCode/tags.xlsx
+++ b/LeetCode/tags.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11213"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/randy/go/src/lightsinger.life/algorithm/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFD95F8-EE5E-3C46-9C83-C6CC3714240D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D0C7B5-0F18-AE47-BCCC-FB39C89B5B67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>map</t>
   </si>
@@ -40,6 +40,27 @@
   </si>
   <si>
     <t>Sliding Windows</t>
+  </si>
+  <si>
+    <t>Palindrome</t>
+  </si>
+  <si>
+    <t>strings</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bits</t>
+  </si>
+  <si>
+    <t>6,8，10</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>Too Hard</t>
+  </si>
+  <si>
+    <t>Greedy</t>
   </si>
 </sst>
 </file>
@@ -416,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,11 +458,29 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" t="s">
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" t="s">
         <v>3</v>
       </c>
+      <c r="P1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -454,12 +493,41 @@
       <c r="D2">
         <v>3</v>
       </c>
-      <c r="R2">
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2">
+        <v>10</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="O2">
         <v>4</v>
+      </c>
+      <c r="P2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>